<commit_message>
[Esquemático] Finalização do esquemático e BoM.
</commit_message>
<xml_diff>
--- a/PCB_Project_Source_IoT/Project Outputs for PCB_Project_Source_IoT/PCB_Project_Source_IoT.xlsx
+++ b/PCB_Project_Source_IoT/Project Outputs for PCB_Project_Source_IoT/PCB_Project_Source_IoT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://academicoifrnedu-my.sharepoint.com/personal/joab_s_academico_ifrn_edu_br/Documents/Documents/SourceIoT/PCB_Project_Source_IoT/Project Outputs for PCB_Project_Source_IoT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfalc\OneDrive - IFRN\Documents\SourceIoT\PCB_Project_Source_IoT\Project Outputs for PCB_Project_Source_IoT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{BEAF38AD-BD15-4311-BA0E-80526945821C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{145D96EE-2B2A-4D0F-934B-5CF039C618DE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE64679E-59C4-4C14-B3F2-814038B27C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21897153-7DC8-4A57-8222-6E500058D9CF}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{21897153-7DC8-4A57-8222-6E500058D9CF}"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="166">
   <si>
     <t>Lista de Materiais</t>
   </si>
@@ -126,7 +126,7 @@
     <t>v.0.1</t>
   </si>
   <si>
-    <t>25/10/2024</t>
+    <t>12/11/2024</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -135,16 +135,397 @@
     <t>Designator</t>
   </si>
   <si>
-    <t>#Column Name Error:' Manufacturer Part Number</t>
+    <t>C2, C6, C8, C10</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C7, C9</t>
+  </si>
+  <si>
+    <t>CONN1</t>
+  </si>
+  <si>
+    <t>D1, D3, D7, D13, D14</t>
+  </si>
+  <si>
+    <t>D2, D15</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5, D6, D10, D11, D12</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D16</t>
+  </si>
+  <si>
+    <t>J1, J4, J5, J8</t>
+  </si>
+  <si>
+    <t>J2, J3, J6, J7</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>R1, R7</t>
+  </si>
+  <si>
+    <t>R2, R6, R10, R14, R15</t>
+  </si>
+  <si>
+    <t>R3, R8, R16</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>T1, T4</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>CL21B104KACNNNC</t>
+  </si>
+  <si>
+    <t>CL21A226MAYNNNE</t>
+  </si>
+  <si>
+    <t>CL31A106KBHNNNE</t>
+  </si>
+  <si>
+    <t>C2012X5R1E475K125AB</t>
+  </si>
+  <si>
+    <t>TSW-101-07-G-D</t>
+  </si>
+  <si>
+    <t>LTST-C170GKT</t>
+  </si>
+  <si>
+    <t>MMSZ5245B-TP</t>
+  </si>
+  <si>
+    <t>SMBJ28CAQ-13-F</t>
+  </si>
+  <si>
+    <t>MBR120VLSFT1G</t>
+  </si>
+  <si>
+    <t>SMAJ5.0A-13-F</t>
+  </si>
+  <si>
+    <t>LTST-C171TBKT</t>
+  </si>
+  <si>
+    <t>SMBJ6.0CA-TR</t>
+  </si>
+  <si>
+    <t>5447861</t>
+  </si>
+  <si>
+    <t>5444262</t>
+  </si>
+  <si>
+    <t>1255AY-4R7M=P3</t>
+  </si>
+  <si>
+    <t>CRGCQ0805F100K</t>
+  </si>
+  <si>
+    <t>CRGCQ0805J470R</t>
+  </si>
+  <si>
+    <t>RC0805FR-0710KL</t>
+  </si>
+  <si>
+    <t>RC0805FR-071KL</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF2001V</t>
+  </si>
+  <si>
+    <t>RC0805FR-071ML</t>
+  </si>
+  <si>
+    <t>RC0805FR-07270KL</t>
+  </si>
+  <si>
+    <t>RC0805FR-0716KL</t>
+  </si>
+  <si>
+    <t>RC0805FR-13330KL</t>
+  </si>
+  <si>
+    <t>DMP4065S-7</t>
+  </si>
+  <si>
+    <t>DDTC143ZCA-7-F</t>
+  </si>
+  <si>
+    <t>PJA3415_R1_00001</t>
+  </si>
+  <si>
+    <t>AP63205WU-7</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OT</t>
+  </si>
+  <si>
+    <t>TLV7031QDBVRQ1</t>
+  </si>
+  <si>
+    <t>LM4041DYM3-1.2-TR</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t>CAP CER 0.1UF 25V X7R 0805</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 25V X5R 0805</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 50V X5R 1206</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 25V X5R 0805</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 2POS</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR SMD</t>
+  </si>
+  <si>
+    <t>DIODE ZENER 15V 500MW SOD123</t>
+  </si>
+  <si>
+    <t>TVS DIODE 28VWM 45.4VC SMB</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 20V 1A SOD123FL</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5VWM 9.2VC SMA</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR CHIP SMD</t>
+  </si>
+  <si>
+    <t>TVS DIODE 6VWM 10.3VC SMB</t>
+  </si>
+  <si>
+    <t>TERM BLOCK PLUG 2POS STR 3.81MM</t>
+  </si>
+  <si>
+    <t>TERM BLOCK HDR 2POS 90DEG 3.81MM</t>
+  </si>
+  <si>
+    <t>FIXED IND 4.7UH 4A 23 MOHM SMD</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES 470 OHM 5% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES 1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES 1M OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES 270K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES 16K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RES 330K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 40V 2.4A SOT23</t>
+  </si>
+  <si>
+    <t>TRANS PREBIAS NPN 200MW SOT23-3</t>
+  </si>
+  <si>
+    <t>MOSFET P-CHANNEL 20V 4A SOT23</t>
+  </si>
+  <si>
+    <t>IC REG BUCK 5V 2A TSOT23-6</t>
+  </si>
+  <si>
+    <t>IC BATT CNTL LI-ION 1CEL SOT23-5</t>
+  </si>
+  <si>
+    <t>AUTOMOTIVE NANO POWER COMPARATOR</t>
+  </si>
+  <si>
+    <t>IC VREF SHUNT 1% SOT23-3</t>
+  </si>
+  <si>
     <t>Supplier 1</t>
   </si>
   <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
     <t>Supplier Part Number 1</t>
+  </si>
+  <si>
+    <t>1276-1099-1-ND</t>
+  </si>
+  <si>
+    <t>1276-CL21A226MAYNNNECT-ND</t>
+  </si>
+  <si>
+    <t>1276-2876-1-ND</t>
+  </si>
+  <si>
+    <t>445-4116-1-ND</t>
+  </si>
+  <si>
+    <t>SAM1028-01-ND</t>
+  </si>
+  <si>
+    <t>160-1179-1-ND</t>
+  </si>
+  <si>
+    <t>MMSZ5245B-TPMSCT-ND</t>
+  </si>
+  <si>
+    <t>SMBJ28CAQ-13-FDICT-ND</t>
+  </si>
+  <si>
+    <t>MBR120VLSFT1GOSCT-ND</t>
+  </si>
+  <si>
+    <t>SMAJ5.0A-E3/61GICT-ND</t>
+  </si>
+  <si>
+    <t>160-1645-1-ND</t>
+  </si>
+  <si>
+    <t>497-7454-1-ND</t>
+  </si>
+  <si>
+    <t>277-11343-ND</t>
+  </si>
+  <si>
+    <t>277-11313-ND</t>
+  </si>
+  <si>
+    <t>490-10812-1-ND</t>
+  </si>
+  <si>
+    <t>A129773CT-ND</t>
+  </si>
+  <si>
+    <t>A130132CT-ND</t>
+  </si>
+  <si>
+    <t>603-RC0805FR-0710KL</t>
+  </si>
+  <si>
+    <t>311-1.00KCRCT-ND</t>
+  </si>
+  <si>
+    <t>P2.00KCCT-ND</t>
+  </si>
+  <si>
+    <t>311-1.00MCRCT-ND</t>
+  </si>
+  <si>
+    <t>603-RC0805FR-07270KL</t>
+  </si>
+  <si>
+    <t>311-16.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>13-RC0805FR-13330KLCT-ND</t>
+  </si>
+  <si>
+    <t>DMP4065S-7DICT-ND</t>
+  </si>
+  <si>
+    <t>1727-3045-1-ND</t>
+  </si>
+  <si>
+    <t>3757-PJA3415_R1_00001CT-ND</t>
+  </si>
+  <si>
+    <t>AP63205WU-7DICT-ND</t>
+  </si>
+  <si>
+    <t>MCP73831T-2ACI/OTCT-ND</t>
+  </si>
+  <si>
+    <t>296-TLV7031QDBVRQ1CT-ND</t>
+  </si>
+  <si>
+    <t>576-2572-1-ND</t>
   </si>
   <si>
     <t>Supplier Stock 1</t>
@@ -458,35 +839,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -635,7 +1016,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -932,30 +1313,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B497636F-CE8D-4C1D-965C-5F55973BFF0E}">
   <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:L16"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" hidden="1"/>
+    <col min="11" max="11" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.109375" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
@@ -967,7 +1348,7 @@
       <c r="J1" s="48"/>
       <c r="K1" s="48"/>
     </row>
-    <row r="5" spans="2:11" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:11" ht="33" x14ac:dyDescent="0.6">
       <c r="B5" s="47" t="s">
         <v>0</v>
       </c>
@@ -981,71 +1362,71 @@
       <c r="J5" s="47"/>
       <c r="K5" s="47"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="49" t="s">
+      <c r="C6" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="50"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="50"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="50"/>
-      <c r="K9" s="50"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1059,7 +1440,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
@@ -1070,88 +1451,1066 @@
         <v>31</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>34</v>
+        <v>127</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>37</v>
+        <v>164</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="19">
         <f>ROW(B13)-ROW($B$12)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="19">
+        <v>4</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="I13" s="19">
+        <v>329324</v>
+      </c>
+      <c r="J13" s="21">
+        <v>3.1E-2</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="19">
-        <f t="shared" ref="B14:B15" si="0">ROW(B14)-ROW($B$12)</f>
+        <f t="shared" ref="B14:B43" si="0">ROW(B14)-ROW($B$12)</f>
         <v>2</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="19">
+        <v>2</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I14" s="19">
+        <v>900030</v>
+      </c>
+      <c r="J14" s="21">
+        <v>0.26</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="19">
+        <f>ROW(B15)-ROW($B$12)</f>
+        <v>3</v>
+      </c>
+      <c r="C15" s="19">
+        <v>1</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="I15" s="19">
+        <v>1103273</v>
+      </c>
+      <c r="J15" s="21">
+        <v>0.36</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="19">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C16" s="19">
+        <v>2</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="I16" s="19">
+        <v>2068027</v>
+      </c>
+      <c r="J16" s="21">
+        <v>0.27</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="19">
+        <f>ROW(B17)-ROW($B$12)</f>
+        <v>5</v>
+      </c>
+      <c r="C17" s="19">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="I17" s="19">
+        <v>3845</v>
+      </c>
+      <c r="J17" s="21">
+        <v>0.69</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B18" s="19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C18" s="19">
+        <v>5</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="I18" s="19">
+        <v>648472</v>
+      </c>
+      <c r="J18" s="21">
+        <v>0.24</v>
+      </c>
+      <c r="K18" s="21">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B19" s="19">
+        <f>ROW(B19)-ROW($B$12)</f>
+        <v>7</v>
+      </c>
+      <c r="C19" s="19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="I19" s="19">
+        <v>599861</v>
+      </c>
+      <c r="J19" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B20" s="19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C20" s="19">
+        <v>1</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="I20" s="19">
+        <v>70366</v>
+      </c>
+      <c r="J20" s="21">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="K20" s="21">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B21" s="19">
+        <f>ROW(B21)-ROW($B$12)</f>
+        <v>9</v>
+      </c>
+      <c r="C21" s="19">
+        <v>5</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="I21" s="19">
+        <v>39177</v>
+      </c>
+      <c r="J21" s="21">
+        <v>0.41</v>
+      </c>
+      <c r="K21" s="21">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="19">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C22" s="19">
+        <v>1</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="G22" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="19">
+        <v>377634</v>
+      </c>
+      <c r="J22" s="21">
+        <v>0.22</v>
+      </c>
+      <c r="K22" s="21">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B23" s="19">
+        <f>ROW(B23)-ROW($B$12)</f>
+        <v>11</v>
+      </c>
+      <c r="C23" s="19">
+        <v>1</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="I23" s="19">
+        <v>30651</v>
+      </c>
+      <c r="J23" s="21">
+        <v>0.32</v>
+      </c>
+      <c r="K23" s="21">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="19">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" s="19">
+        <v>6349</v>
+      </c>
+      <c r="J24" s="21">
+        <v>0.47</v>
+      </c>
+      <c r="K24" s="21">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="19">
+        <f>ROW(B25)-ROW($B$12)</f>
+        <v>13</v>
+      </c>
+      <c r="C25" s="19">
+        <v>4</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="G25" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="I25" s="19">
+        <v>112594</v>
+      </c>
+      <c r="J25" s="21">
+        <v>1.34</v>
+      </c>
+      <c r="K25" s="21">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="19">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C26" s="19">
+        <v>4</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="I26" s="19">
+        <v>197636</v>
+      </c>
+      <c r="J26" s="21">
+        <v>0.7</v>
+      </c>
+      <c r="K26" s="21">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B27" s="19">
+        <f>ROW(B27)-ROW($B$12)</f>
+        <v>15</v>
+      </c>
+      <c r="C27" s="19">
+        <v>1</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="I27" s="19">
+        <v>134310</v>
+      </c>
+      <c r="J27" s="21">
+        <v>0.47</v>
+      </c>
+      <c r="K27" s="21">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B28" s="19">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C28" s="19">
+        <v>2</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="19">
+        <v>238357</v>
+      </c>
+      <c r="J28" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K28" s="21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="19">
+        <f>ROW(B29)-ROW($B$12)</f>
+        <v>17</v>
+      </c>
+      <c r="C29" s="19">
+        <v>5</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="I29" s="19">
+        <v>814565</v>
+      </c>
+      <c r="J29" s="21">
+        <v>2.7E-2</v>
+      </c>
+      <c r="K29" s="21">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B30" s="19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C30" s="19">
         <v>3</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="23">
-        <f>SUM(C13:C15)</f>
-        <v>0</v>
-      </c>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="24">
-        <f>SUM(K13:K15)</f>
-        <v>0</v>
+      <c r="D30" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="H30" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I30" s="19">
+        <v>1732265</v>
+      </c>
+      <c r="J30" s="21">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="K30" s="21">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="19">
+        <f>ROW(B31)-ROW($B$12)</f>
+        <v>19</v>
+      </c>
+      <c r="C31" s="19">
+        <v>1</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H31" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="I31" s="19">
+        <v>1457562</v>
+      </c>
+      <c r="J31" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K31" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B32" s="19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C32" s="19">
+        <v>1</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="I32" s="19">
+        <v>134954</v>
+      </c>
+      <c r="J32" s="21">
+        <v>0.11</v>
+      </c>
+      <c r="K32" s="21">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B33" s="19">
+        <f>ROW(B33)-ROW($B$12)</f>
+        <v>21</v>
+      </c>
+      <c r="C33" s="19">
+        <v>1</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="I33" s="19">
+        <v>91345</v>
+      </c>
+      <c r="J33" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K33" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B34" s="19">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C34" s="19">
+        <v>1</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="I34" s="19">
+        <v>272</v>
+      </c>
+      <c r="J34" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K34" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="19">
+        <f>ROW(B35)-ROW($B$12)</f>
+        <v>23</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="I35" s="19">
+        <v>149233</v>
+      </c>
+      <c r="J35" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K35" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="19">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C36" s="19">
+        <v>1</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="I36" s="19">
+        <v>22156</v>
+      </c>
+      <c r="J36" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K36" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B37" s="19">
+        <f>ROW(B37)-ROW($B$12)</f>
+        <v>25</v>
+      </c>
+      <c r="C37" s="19">
+        <v>2</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="I37" s="19">
+        <v>31893</v>
+      </c>
+      <c r="J37" s="21">
+        <v>0.32</v>
+      </c>
+      <c r="K37" s="21">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B38" s="19">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C38" s="19">
+        <v>1</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I38" s="19">
+        <v>181441</v>
+      </c>
+      <c r="J38" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="K38" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B39" s="19">
+        <f>ROW(B39)-ROW($B$12)</f>
+        <v>27</v>
+      </c>
+      <c r="C39" s="19">
+        <v>1</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="I39" s="19">
+        <v>6943</v>
+      </c>
+      <c r="J39" s="21">
+        <v>0.23</v>
+      </c>
+      <c r="K39" s="21">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B40" s="19">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C40" s="19">
+        <v>1</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="I40" s="19">
+        <v>16299</v>
+      </c>
+      <c r="J40" s="21">
+        <v>1.32</v>
+      </c>
+      <c r="K40" s="21">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B41" s="19">
+        <f>ROW(B41)-ROW($B$12)</f>
+        <v>29</v>
+      </c>
+      <c r="C41" s="19">
+        <v>1</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="I41" s="19">
+        <v>94379</v>
+      </c>
+      <c r="J41" s="21">
+        <v>0.76</v>
+      </c>
+      <c r="K41" s="21">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B42" s="19">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C42" s="19">
+        <v>1</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="I42" s="19">
+        <v>14235</v>
+      </c>
+      <c r="J42" s="21">
+        <v>0.72</v>
+      </c>
+      <c r="K42" s="21">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="19">
+        <f>ROW(B43)-ROW($B$12)</f>
+        <v>31</v>
+      </c>
+      <c r="C43" s="19">
+        <v>1</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="I43" s="19">
+        <v>40272</v>
+      </c>
+      <c r="J43" s="21">
+        <v>0.36</v>
+      </c>
+      <c r="K43" s="21">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+      <c r="C44" s="23">
+        <f>SUM(C13:C43)</f>
+        <v>59</v>
+      </c>
+      <c r="D44" s="50"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="24">
+        <f>SUM(K13:K43)</f>
+        <v>21.180000000000014</v>
       </c>
     </row>
   </sheetData>
@@ -1159,12 +2518,12 @@
     <mergeCell ref="B5:K5"/>
     <mergeCell ref="B1:K1"/>
     <mergeCell ref="C9:K9"/>
-    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D44:J44"/>
     <mergeCell ref="C8:K8"/>
     <mergeCell ref="C7:K7"/>
     <mergeCell ref="C6:K6"/>
   </mergeCells>
-  <conditionalFormatting sqref="B13:K15">
+  <conditionalFormatting sqref="B13:K43">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$I13&lt;$C13</formula>
     </cfRule>
@@ -1183,35 +2542,35 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
     <col min="4" max="4" width="2" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="3.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="3.109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="15" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="28" hidden="1"/>
-    <col min="9" max="9" width="26.7109375" hidden="1"/>
-    <col min="10" max="10" width="26.140625" hidden="1"/>
-    <col min="11" max="16362" width="8.85546875" hidden="1"/>
-    <col min="16364" max="16384" width="8.85546875" hidden="1"/>
+    <col min="9" max="9" width="26.6640625" hidden="1"/>
+    <col min="10" max="10" width="26.109375" hidden="1"/>
+    <col min="11" max="16362" width="8.88671875" hidden="1"/>
+    <col min="16364" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:9" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:9" ht="33" x14ac:dyDescent="0.3">
+      <c r="A8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
@@ -1219,7 +2578,7 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
       <c r="B9" s="27"/>
       <c r="C9" s="27"/>
@@ -1228,20 +2587,20 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -1256,17 +2615,17 @@
       <c r="H11" s="30"/>
       <c r="I11" s="30"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="8">
-        <f>BoM!K16</f>
-        <v>0</v>
+        <f>BoM!K44</f>
+        <v>21.180000000000014</v>
       </c>
       <c r="C12" s="9">
         <f t="shared" ref="C12:C17" si="0">B12*$B$22</f>
-        <v>0</v>
+        <v>119.38742400000008</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="38"/>
@@ -1275,7 +2634,7 @@
       <c r="H12" s="30"/>
       <c r="I12" s="30"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1293,17 +2652,17 @@
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="8">
         <f>0.6*SUM(B12:B13)</f>
-        <v>24</v>
+        <v>36.708000000000006</v>
       </c>
       <c r="C14" s="9">
         <f t="shared" si="0"/>
-        <v>135.28319999999999</v>
+        <v>206.91565440000002</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="38"/>
@@ -1312,24 +2671,24 @@
       <c r="H14" s="5"/>
       <c r="I14" s="31"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="8">
         <f>SUM(B12:B14)*0.18/0.82</f>
-        <v>14.048780487804878</v>
+        <v>21.487609756097566</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" si="0"/>
-        <v>79.190165853658542</v>
+        <v>121.12135867317076</v>
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="38"/>
       <c r="F15" s="37"/>
       <c r="G15" s="38"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1345,30 +2704,30 @@
       <c r="F16" s="37"/>
       <c r="G16" s="38"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="15">
         <f>SUM(B14:B16)</f>
-        <v>54.918780487804881</v>
+        <v>75.065609756097572</v>
       </c>
       <c r="C17" s="16">
         <f t="shared" si="0"/>
-        <v>309.56618185365858</v>
+        <v>423.12982907317081</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="38"/>
       <c r="F17" s="37"/>
       <c r="G17" s="38"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A19" s="54" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:9" ht="33" x14ac:dyDescent="0.6">
+      <c r="A19" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="56"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
@@ -1376,7 +2735,7 @@
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1385,10 +2744,10 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="e">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="str">
         <f ca="1">"USD &lt;-&gt; BRL (" &amp; TEXT(TODAY(),"DD/MM/AA") &amp;")"</f>
-        <v>#VALUE!</v>
+        <v>USD &lt;-&gt; BRL (12/11/24)</v>
       </c>
       <c r="B21" s="33">
         <v>5.42</v>
@@ -1396,7 +2755,7 @@
       <c r="C21" s="34"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>16</v>
       </c>
@@ -1407,85 +2766,85 @@
       <c r="C22" s="36"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="54" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="58"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C23" s="55"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="8">
         <f>SUM(B12:B13)</f>
-        <v>40</v>
+        <v>61.180000000000014</v>
       </c>
       <c r="C24" s="9">
         <f>B24*$B$22</f>
-        <v>225.47200000000001</v>
+        <v>344.8594240000001</v>
       </c>
       <c r="D24" s="37"/>
       <c r="E24" s="38"/>
       <c r="F24" s="37"/>
       <c r="G24" s="38"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="8">
         <f>SUM(B14:B16)</f>
-        <v>54.918780487804881</v>
+        <v>75.065609756097572</v>
       </c>
       <c r="C25" s="9">
         <f>B25*$B$22</f>
-        <v>309.56618185365858</v>
+        <v>423.12982907317081</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="38"/>
       <c r="F25" s="37"/>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="28">
         <f>SUM(B24:B25)</f>
-        <v>94.918780487804881</v>
+        <v>136.24560975609759</v>
       </c>
       <c r="C26" s="26">
         <f t="shared" ref="C26" si="1">SUM(C24:C25)</f>
-        <v>535.03818185365856</v>
+        <v>767.98925307317086</v>
       </c>
       <c r="D26" s="39"/>
       <c r="E26" s="40"/>
       <c r="F26" s="39"/>
       <c r="G26" s="40"/>
     </row>
-    <row r="27" spans="1:9" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
+    <row r="27" spans="1:9" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
+      <c r="B27" s="57"/>
+      <c r="C27" s="57"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="44"/>
       <c r="G27" s="45"/>
     </row>
-    <row r="28" spans="1:9" s="41" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="55" t="s">
+    <row r="28" spans="1:9" s="41" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="57"/>
       <c r="D28" s="46"/>
       <c r="E28" s="46"/>
       <c r="F28" s="43"/>
@@ -1493,7 +2852,7 @@
       <c r="H28" s="42"/>
       <c r="I28" s="42"/>
     </row>
-    <row r="64" spans="4:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="4:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="D64" t="s">
         <v>17</v>
       </c>
@@ -1503,16 +2862,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
@@ -1520,26 +2879,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="eafd81bd-aa47-44fe-a879-d8b0a59d073f" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="67754bcf-640a-45dc-a4a1-3295cc8f1c13">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100983A3410C182AB469BFD6543519C0FE4" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="2fe405e9385892723840c96a6d735dcf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="67754bcf-640a-45dc-a4a1-3295cc8f1c13" xmlns:ns3="eafd81bd-aa47-44fe-a879-d8b0a59d073f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e3278376455a019c4f3e06f3cbff1cf" ns2:_="" ns3:_="">
     <xsd:import namespace="67754bcf-640a-45dc-a4a1-3295cc8f1c13"/>
@@ -1742,26 +3081,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ECEDFC9-7F99-4013-85DF-09F0F86F7B6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="eafd81bd-aa47-44fe-a879-d8b0a59d073f"/>
-    <ds:schemaRef ds:uri="67754bcf-640a-45dc-a4a1-3295cc8f1c13"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B4973F1-FB21-417F-AF6C-D9174DD308EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="eafd81bd-aa47-44fe-a879-d8b0a59d073f" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="67754bcf-640a-45dc-a4a1-3295cc8f1c13">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A013DF8D-4E7A-4B00-A047-BE5897B9F82D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1778,4 +3118,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B4973F1-FB21-417F-AF6C-D9174DD308EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ECEDFC9-7F99-4013-85DF-09F0F86F7B6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="eafd81bd-aa47-44fe-a879-d8b0a59d073f"/>
+    <ds:schemaRef ds:uri="67754bcf-640a-45dc-a4a1-3295cc8f1c13"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[Libraries e Esquemático] Atualização nas bibliotecas e camadas e finalização do esquemático
</commit_message>
<xml_diff>
--- a/PCB_Project_Source_IoT/Project Outputs for PCB_Project_Source_IoT/PCB_Project_Source_IoT.xlsx
+++ b/PCB_Project_Source_IoT/Project Outputs for PCB_Project_Source_IoT/PCB_Project_Source_IoT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfalc\OneDrive - IFRN\Documents\SourceIoT\PCB_Project_Source_IoT\Project Outputs for PCB_Project_Source_IoT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DE64679E-59C4-4C14-B3F2-814038B27C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEC13FF4-201D-4C18-B786-6EBAD964D711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{21897153-7DC8-4A57-8222-6E500058D9CF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{21897153-7DC8-4A57-8222-6E500058D9CF}"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
     <t>v.0.1</t>
   </si>
   <si>
-    <t>12/11/2024</t>
+    <t>30/11/2024</t>
   </si>
   <si>
     <t>Quantity</t>
@@ -1496,13 +1496,13 @@
         <v>132</v>
       </c>
       <c r="I13" s="19">
-        <v>329324</v>
+        <v>310523</v>
       </c>
       <c r="J13" s="21">
-        <v>3.1E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K13" s="21">
-        <v>0.31</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1529,13 +1529,13 @@
         <v>133</v>
       </c>
       <c r="I14" s="19">
-        <v>900030</v>
+        <v>752073</v>
       </c>
       <c r="J14" s="21">
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
       <c r="K14" s="21">
-        <v>0.52</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1562,13 +1562,13 @@
         <v>134</v>
       </c>
       <c r="I15" s="19">
-        <v>1103273</v>
+        <v>1069929</v>
       </c>
       <c r="J15" s="21">
-        <v>0.36</v>
+        <v>0.26</v>
       </c>
       <c r="K15" s="21">
-        <v>0.36</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1595,7 +1595,7 @@
         <v>135</v>
       </c>
       <c r="I16" s="19">
-        <v>2068027</v>
+        <v>2065446</v>
       </c>
       <c r="J16" s="21">
         <v>0.27</v>
@@ -1628,13 +1628,13 @@
         <v>136</v>
       </c>
       <c r="I17" s="19">
-        <v>3845</v>
+        <v>4011</v>
       </c>
       <c r="J17" s="21">
-        <v>0.69</v>
+        <v>0.51</v>
       </c>
       <c r="K17" s="21">
-        <v>0.69</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="18" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1661,7 +1661,7 @@
         <v>137</v>
       </c>
       <c r="I18" s="19">
-        <v>648472</v>
+        <v>591372</v>
       </c>
       <c r="J18" s="21">
         <v>0.24</v>
@@ -1694,7 +1694,7 @@
         <v>138</v>
       </c>
       <c r="I19" s="19">
-        <v>599861</v>
+        <v>571402</v>
       </c>
       <c r="J19" s="21">
         <v>0.1</v>
@@ -1727,7 +1727,7 @@
         <v>139</v>
       </c>
       <c r="I20" s="19">
-        <v>70366</v>
+        <v>70179</v>
       </c>
       <c r="J20" s="21">
         <v>0.28999999999999998</v>
@@ -1760,7 +1760,7 @@
         <v>140</v>
       </c>
       <c r="I21" s="19">
-        <v>39177</v>
+        <v>34078</v>
       </c>
       <c r="J21" s="21">
         <v>0.41</v>
@@ -1793,7 +1793,7 @@
         <v>141</v>
       </c>
       <c r="I22" s="19">
-        <v>377634</v>
+        <v>373124</v>
       </c>
       <c r="J22" s="21">
         <v>0.22</v>
@@ -1826,7 +1826,7 @@
         <v>142</v>
       </c>
       <c r="I23" s="19">
-        <v>30651</v>
+        <v>12486</v>
       </c>
       <c r="J23" s="21">
         <v>0.32</v>
@@ -1859,7 +1859,7 @@
         <v>143</v>
       </c>
       <c r="I24" s="19">
-        <v>6349</v>
+        <v>3849</v>
       </c>
       <c r="J24" s="21">
         <v>0.47</v>
@@ -1892,7 +1892,7 @@
         <v>144</v>
       </c>
       <c r="I25" s="19">
-        <v>112594</v>
+        <v>112312</v>
       </c>
       <c r="J25" s="21">
         <v>1.34</v>
@@ -1925,7 +1925,7 @@
         <v>145</v>
       </c>
       <c r="I26" s="19">
-        <v>197636</v>
+        <v>196590</v>
       </c>
       <c r="J26" s="21">
         <v>0.7</v>
@@ -1958,7 +1958,7 @@
         <v>146</v>
       </c>
       <c r="I27" s="19">
-        <v>134310</v>
+        <v>129802</v>
       </c>
       <c r="J27" s="21">
         <v>0.47</v>
@@ -1991,7 +1991,7 @@
         <v>147</v>
       </c>
       <c r="I28" s="19">
-        <v>238357</v>
+        <v>237873</v>
       </c>
       <c r="J28" s="21">
         <v>0.1</v>
@@ -2024,7 +2024,7 @@
         <v>148</v>
       </c>
       <c r="I29" s="19">
-        <v>814565</v>
+        <v>806449</v>
       </c>
       <c r="J29" s="21">
         <v>2.7E-2</v>
@@ -2057,7 +2057,7 @@
         <v>149</v>
       </c>
       <c r="I30" s="19">
-        <v>1732265</v>
+        <v>1439925</v>
       </c>
       <c r="J30" s="21">
         <v>1.7000000000000001E-2</v>
@@ -2090,7 +2090,7 @@
         <v>150</v>
       </c>
       <c r="I31" s="19">
-        <v>1457562</v>
+        <v>1286489</v>
       </c>
       <c r="J31" s="21">
         <v>0.1</v>
@@ -2123,7 +2123,7 @@
         <v>151</v>
       </c>
       <c r="I32" s="19">
-        <v>134954</v>
+        <v>117776</v>
       </c>
       <c r="J32" s="21">
         <v>0.11</v>
@@ -2156,7 +2156,7 @@
         <v>152</v>
       </c>
       <c r="I33" s="19">
-        <v>91345</v>
+        <v>181075</v>
       </c>
       <c r="J33" s="21">
         <v>0.1</v>
@@ -2189,7 +2189,7 @@
         <v>153</v>
       </c>
       <c r="I34" s="19">
-        <v>272</v>
+        <v>29900</v>
       </c>
       <c r="J34" s="21">
         <v>0.1</v>
@@ -2222,7 +2222,7 @@
         <v>154</v>
       </c>
       <c r="I35" s="19">
-        <v>149233</v>
+        <v>147953</v>
       </c>
       <c r="J35" s="21">
         <v>0.1</v>
@@ -2288,7 +2288,7 @@
         <v>156</v>
       </c>
       <c r="I37" s="19">
-        <v>31893</v>
+        <v>30248</v>
       </c>
       <c r="J37" s="21">
         <v>0.32</v>
@@ -2321,13 +2321,13 @@
         <v>157</v>
       </c>
       <c r="I38" s="19">
-        <v>181441</v>
+        <v>11141</v>
       </c>
       <c r="J38" s="21">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="K38" s="21">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="39" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -2354,13 +2354,13 @@
         <v>158</v>
       </c>
       <c r="I39" s="19">
-        <v>6943</v>
+        <v>18943</v>
       </c>
       <c r="J39" s="21">
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
       <c r="K39" s="21">
-        <v>0.23</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="40" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -2387,7 +2387,7 @@
         <v>159</v>
       </c>
       <c r="I40" s="19">
-        <v>16299</v>
+        <v>29348</v>
       </c>
       <c r="J40" s="21">
         <v>1.32</v>
@@ -2420,7 +2420,7 @@
         <v>160</v>
       </c>
       <c r="I41" s="19">
-        <v>94379</v>
+        <v>92195</v>
       </c>
       <c r="J41" s="21">
         <v>0.76</v>
@@ -2453,7 +2453,7 @@
         <v>161</v>
       </c>
       <c r="I42" s="19">
-        <v>14235</v>
+        <v>15236</v>
       </c>
       <c r="J42" s="21">
         <v>0.72</v>
@@ -2486,7 +2486,7 @@
         <v>162</v>
       </c>
       <c r="I43" s="19">
-        <v>40272</v>
+        <v>39272</v>
       </c>
       <c r="J43" s="21">
         <v>0.36</v>
@@ -2510,7 +2510,7 @@
       <c r="J44" s="52"/>
       <c r="K44" s="24">
         <f>SUM(K13:K43)</f>
-        <v>21.180000000000014</v>
+        <v>20.770000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2621,11 +2621,11 @@
       </c>
       <c r="B12" s="8">
         <f>BoM!K44</f>
-        <v>21.180000000000014</v>
+        <v>20.770000000000003</v>
       </c>
       <c r="C12" s="9">
         <f t="shared" ref="C12:C17" si="0">B12*$B$22</f>
-        <v>119.38742400000008</v>
+        <v>117.07633600000001</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="38"/>
@@ -2658,11 +2658,11 @@
       </c>
       <c r="B14" s="8">
         <f>0.6*SUM(B12:B13)</f>
-        <v>36.708000000000006</v>
+        <v>36.462000000000003</v>
       </c>
       <c r="C14" s="9">
         <f t="shared" si="0"/>
-        <v>206.91565440000002</v>
+        <v>205.52900160000002</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="38"/>
@@ -2677,11 +2677,11 @@
       </c>
       <c r="B15" s="8">
         <f>SUM(B12:B14)*0.18/0.82</f>
-        <v>21.487609756097566</v>
+        <v>21.343609756097564</v>
       </c>
       <c r="C15" s="9">
         <f t="shared" si="0"/>
-        <v>121.12135867317076</v>
+        <v>120.30965947317075</v>
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="38"/>
@@ -2710,11 +2710,11 @@
       </c>
       <c r="B17" s="15">
         <f>SUM(B14:B16)</f>
-        <v>75.065609756097572</v>
+        <v>74.675609756097572</v>
       </c>
       <c r="C17" s="16">
         <f t="shared" si="0"/>
-        <v>423.12982907317081</v>
+        <v>420.93147707317081</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="38"/>
@@ -2745,9 +2745,9 @@
       <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="str">
+      <c r="A21" s="11" t="e">
         <f ca="1">"USD &lt;-&gt; BRL (" &amp; TEXT(TODAY(),"DD/MM/AA") &amp;")"</f>
-        <v>USD &lt;-&gt; BRL (12/11/24)</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B21" s="33">
         <v>5.42</v>
@@ -2783,11 +2783,11 @@
       </c>
       <c r="B24" s="8">
         <f>SUM(B12:B13)</f>
-        <v>61.180000000000014</v>
+        <v>60.77</v>
       </c>
       <c r="C24" s="9">
         <f>B24*$B$22</f>
-        <v>344.8594240000001</v>
+        <v>342.54833600000001</v>
       </c>
       <c r="D24" s="37"/>
       <c r="E24" s="38"/>
@@ -2800,11 +2800,11 @@
       </c>
       <c r="B25" s="8">
         <f>SUM(B14:B16)</f>
-        <v>75.065609756097572</v>
+        <v>74.675609756097572</v>
       </c>
       <c r="C25" s="9">
         <f>B25*$B$22</f>
-        <v>423.12982907317081</v>
+        <v>420.93147707317081</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="38"/>
@@ -2817,11 +2817,11 @@
       </c>
       <c r="B26" s="28">
         <f>SUM(B24:B25)</f>
-        <v>136.24560975609759</v>
+        <v>135.44560975609758</v>
       </c>
       <c r="C26" s="26">
         <f t="shared" ref="C26" si="1">SUM(C24:C25)</f>
-        <v>767.98925307317086</v>
+        <v>763.47981307317082</v>
       </c>
       <c r="D26" s="39"/>
       <c r="E26" s="40"/>

</xml_diff>